<commit_message>
feat(HES-712): For all P2P meters IP and PORT fields should be replaced with a HOSTNAME, similar to what has been done for DC's
</commit_message>
<xml_diff>
--- a/src/assets/files/meter-import.xlsx
+++ b/src/assets/files/meter-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\epoint-hes-ui\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDA7762-6F63-444A-BAEE-C911ED82A377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBA1D7B-9C67-4474-B023-267A1D1EDFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="165" windowWidth="28800" windowHeight="15435" xr2:uid="{AD0087DB-B3CF-424F-A3B1-CF03AF7D857B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD0087DB-B3CF-424F-A3B1-CF03AF7D857B}"/>
   </bookViews>
   <sheets>
     <sheet name="Import data" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>AuthenticationType</t>
   </si>
   <si>
-    <t>Ip</t>
-  </si>
-  <si>
     <t>Port</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>PublicServerAddress</t>
+  </si>
+  <si>
+    <t>Hostname</t>
   </si>
 </sst>
 </file>
@@ -343,6 +343,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,11 +360,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad 2" xfId="2" xr:uid="{6EBCB6DF-5D5B-44F9-B8EE-D92487182617}"/>
@@ -679,23 +679,23 @@
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -715,95 +715,95 @@
     <col min="29" max="29" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" style="13"/>
+    <col min="32" max="32" width="9.140625" style="9"/>
     <col min="35" max="36" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="7" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
       <c r="AI1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AJ1" s="3"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="14" t="s">
+      <c r="J2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>4</v>
@@ -812,67 +812,67 @@
         <v>15</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF2" s="15" t="s">
+      <c r="AF2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH2" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="AI2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -910,19 +910,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="A1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -946,7 +946,7 @@
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -954,139 +954,139 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11" t="s">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
feat(HES-1488): Import MBUS configurations
</commit_message>
<xml_diff>
--- a/src/assets/files/meter-import.xlsx
+++ b/src/assets/files/meter-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\epoint-hes-ui\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBA1D7B-9C67-4474-B023-267A1D1EDFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7489B17-8E0A-4F48-81F9-2061B28FA609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD0087DB-B3CF-424F-A3B1-CF03AF7D857B}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{AD0087DB-B3CF-424F-A3B1-CF03AF7D857B}"/>
   </bookViews>
   <sheets>
     <sheet name="Import data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Basic parameters</t>
   </si>
@@ -202,9 +202,6 @@
     <t>G3PLC</t>
   </si>
   <si>
-    <t>MM_BUS</t>
-  </si>
-  <si>
     <t>Protocol</t>
   </si>
   <si>
@@ -224,6 +221,12 @@
   </si>
   <si>
     <t>Hostname</t>
+  </si>
+  <si>
+    <t>Mbus</t>
+  </si>
+  <si>
+    <t>WMBus</t>
   </si>
 </sst>
 </file>
@@ -678,48 +681,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3196B651-1290-44A4-B315-CE8224E7FB1E}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" style="9"/>
+    <col min="32" max="32" width="9.1796875" style="9"/>
     <col min="35" max="36" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -765,7 +768,7 @@
       </c>
       <c r="AJ1" s="3"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -794,13 +797,13 @@
         <v>7</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>16</v>
@@ -836,16 +839,16 @@
         <v>24</v>
       </c>
       <c r="X2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>25</v>
@@ -890,28 +893,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D6A636-8C87-4EAB-8256-8DACB61DD326}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -924,7 +927,7 @@
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -946,14 +949,14 @@
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -978,7 +981,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>39</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
@@ -1021,10 +1024,10 @@
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
@@ -1041,9 +1044,11 @@
         <v>53</v>
       </c>
       <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="K7" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -1058,7 +1063,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
@@ -1073,7 +1078,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
feat(HES-1937): Additional medium types added
</commit_message>
<xml_diff>
--- a/src/assets/files/meter-import.xlsx
+++ b/src/assets/files/meter-import.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26322"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\epoint-hes-ui\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7489B17-8E0A-4F48-81F9-2061B28FA609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A7489B17-8E0A-4F48-81F9-2061B28FA609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19D66320-E9C8-4F21-91BD-0462B70F2F73}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{AD0087DB-B3CF-424F-A3B1-CF03AF7D857B}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{AD0087DB-B3CF-424F-A3B1-CF03AF7D857B}"/>
   </bookViews>
   <sheets>
     <sheet name="Import data" sheetId="1" r:id="rId1"/>
     <sheet name="Data specification" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,205 +37,292 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
   <si>
     <t>Basic parameters</t>
   </si>
   <si>
+    <t>Communication module</t>
+  </si>
+  <si>
+    <t>Extra parameters</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
     <t>Manufacturer</t>
   </si>
   <si>
+    <t>SerialNumber</t>
+  </si>
+  <si>
     <t>ExternalId</t>
   </si>
   <si>
-    <t>SerialNumber</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>MacAddress</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>ParentManufacturer</t>
+  </si>
+  <si>
+    <t>ParentSerialNumber</t>
+  </si>
+  <si>
+    <t>ConfigurationID</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>InterfaceType</t>
+  </si>
+  <si>
+    <t>Hostname</t>
+  </si>
+  <si>
+    <t>Port</t>
   </si>
   <si>
     <t>ReferencingType</t>
   </si>
   <si>
-    <t>InterfaceType</t>
+    <t>AuthenticationType</t>
+  </si>
+  <si>
+    <t>PublicClientLow</t>
+  </si>
+  <si>
+    <t>PublicClientHigh</t>
+  </si>
+  <si>
+    <t>PublicServerLow</t>
+  </si>
+  <si>
+    <t>PublicServerHigh</t>
+  </si>
+  <si>
+    <t>ClientLow</t>
+  </si>
+  <si>
+    <t>ClientHigh</t>
+  </si>
+  <si>
+    <t>ServerLow</t>
+  </si>
+  <si>
+    <t>ServerHigh</t>
+  </si>
+  <si>
+    <t>ClientAddress</t>
+  </si>
+  <si>
+    <t>ServerAddress</t>
+  </si>
+  <si>
+    <t>PublicClientAddress</t>
+  </si>
+  <si>
+    <t>PublicServerAddress</t>
+  </si>
+  <si>
+    <t>IsGateWay</t>
+  </si>
+  <si>
+    <t>PhysicalAddress</t>
+  </si>
+  <si>
+    <t>StartWithRelease</t>
+  </si>
+  <si>
+    <t>LDNAsSystitle</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>PropertyName1</t>
+  </si>
+  <si>
+    <t>PropertyName2</t>
+  </si>
+  <si>
+    <t>Enum values</t>
   </si>
   <si>
     <t>LGZ</t>
   </si>
   <si>
-    <t>ConfigurationID</t>
-  </si>
-  <si>
     <t>HDLC</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>MacAddress</t>
-  </si>
-  <si>
-    <t>ParentManufacturer</t>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>CosemLogicalName</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>G3PLC</t>
+  </si>
+  <si>
+    <t>ISK</t>
+  </si>
+  <si>
+    <t>WRAPPER</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>CosemShortName</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
   <si>
     <t>DLMS</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Communication module</t>
-  </si>
-  <si>
-    <t>AuthenticationType</t>
-  </si>
-  <si>
-    <t>Port</t>
-  </si>
-  <si>
-    <t>PublicClientLow</t>
-  </si>
-  <si>
-    <t>PublicServerLow</t>
-  </si>
-  <si>
-    <t>PublicServerHigh</t>
-  </si>
-  <si>
-    <t>PublicClientHigh</t>
-  </si>
-  <si>
-    <t>ClientLow</t>
-  </si>
-  <si>
-    <t>ClientHigh</t>
-  </si>
-  <si>
-    <t>ServerLow</t>
-  </si>
-  <si>
-    <t>ServerHigh</t>
-  </si>
-  <si>
-    <t>IsGateWay</t>
-  </si>
-  <si>
-    <t>PhysicalAddress</t>
-  </si>
-  <si>
-    <t>StartWithRelease</t>
-  </si>
-  <si>
-    <t>LDNAsSystitle</t>
-  </si>
-  <si>
-    <t>Extra parameters</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>PropertyName1</t>
-  </si>
-  <si>
-    <t>PropertyName2</t>
-  </si>
-  <si>
-    <t>ParentSerialNumber</t>
-  </si>
-  <si>
-    <t>CosemLogicalName</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>ISK</t>
-  </si>
-  <si>
     <t>ESR</t>
   </si>
   <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Mbus</t>
+  </si>
+  <si>
     <t>ELS</t>
   </si>
   <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>HighGMAC</t>
+  </si>
+  <si>
+    <t>WMBus</t>
+  </si>
+  <si>
     <t>SAG</t>
   </si>
   <si>
+    <t>Heat</t>
+  </si>
+  <si>
     <t>KAM</t>
   </si>
   <si>
+    <t>Steam</t>
+  </si>
+  <si>
     <t>SMX</t>
   </si>
   <si>
-    <t>WRAPPER</t>
-  </si>
-  <si>
-    <t>ELECTRICITY</t>
-  </si>
-  <si>
-    <t>WATER</t>
-  </si>
-  <si>
-    <t>GAS</t>
-  </si>
-  <si>
-    <t>HEAT</t>
-  </si>
-  <si>
-    <t>CosemShortName</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>HighGMAC</t>
-  </si>
-  <si>
-    <t>G3PLC</t>
-  </si>
-  <si>
-    <t>Protocol</t>
-  </si>
-  <si>
-    <t>Enum values</t>
-  </si>
-  <si>
-    <t>ClientAddress</t>
-  </si>
-  <si>
-    <t>ServerAddress</t>
-  </si>
-  <si>
-    <t>PublicClientAddress</t>
-  </si>
-  <si>
-    <t>PublicServerAddress</t>
-  </si>
-  <si>
-    <t>Hostname</t>
-  </si>
-  <si>
-    <t>Mbus</t>
-  </si>
-  <si>
-    <t>WMBus</t>
+    <t>WarmWater</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>HeatCostAllocator</t>
+  </si>
+  <si>
+    <t>CompressedAir</t>
+  </si>
+  <si>
+    <t>CoolingRetrun</t>
+  </si>
+  <si>
+    <t>CoolingInlet</t>
+  </si>
+  <si>
+    <t>HeatInlet</t>
+  </si>
+  <si>
+    <t>HeatCooling</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Consumption0</t>
+  </si>
+  <si>
+    <t>Consumption1</t>
+  </si>
+  <si>
+    <t>Consumption2</t>
+  </si>
+  <si>
+    <t>Consumption3</t>
+  </si>
+  <si>
+    <t>Calorific</t>
+  </si>
+  <si>
+    <t>HotWater</t>
+  </si>
+  <si>
+    <t>ColdWater</t>
+  </si>
+  <si>
+    <t>DualRegisterWaterMeter</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>ADConverter</t>
+  </si>
+  <si>
+    <t>GasDetector</t>
+  </si>
+  <si>
+    <t>Breaker</t>
+  </si>
+  <si>
+    <t>CustomerUnit</t>
+  </si>
+  <si>
+    <t>WasteWater</t>
+  </si>
+  <si>
+    <t>Garbage</t>
+  </si>
+  <si>
+    <t>CarbonDioxide</t>
+  </si>
+  <si>
+    <t>Unidirectional</t>
+  </si>
+  <si>
+    <t>Bidirectional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,7 +455,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad 2" xfId="2" xr:uid="{6EBCB6DF-5D5B-44F9-B8EE-D92487182617}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{265E8CEA-DE9E-4F46-9615-8C18A90BAEDF}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -685,44 +774,44 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.1796875" style="9"/>
+    <col min="32" max="32" width="9.140625" style="9"/>
     <col min="35" max="36" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -735,7 +824,7 @@
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
       <c r="J1" s="12" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
@@ -759,123 +848,123 @@
       <c r="AD1" s="12"/>
       <c r="AE1" s="12"/>
       <c r="AF1" s="14" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="AG1" s="14"/>
       <c r="AH1" s="14"/>
       <c r="AI1" s="3" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="AJ1" s="3"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36">
       <c r="A2" s="8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="K2" s="10" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="AF2" s="11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -891,30 +980,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D6A636-8C87-4EAB-8256-8DACB61DD326}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E4" sqref="E4:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="24" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -927,71 +1016,71 @@
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4" s="7" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
@@ -999,63 +1088,65 @@
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="7" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="7" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -1063,14 +1154,16 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11">
       <c r="A9" s="7" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -1078,20 +1171,152 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11">
       <c r="A10" s="7" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="E13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
+      <c r="E21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
+      <c r="E25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
+      <c r="E28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
+      <c r="E29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
feat(HES-1818): DC450 UI enhancements
</commit_message>
<xml_diff>
--- a/src/assets/files/meter-import.xlsx
+++ b/src/assets/files/meter-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\epoint-hes-ui\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A7489B17-8E0A-4F48-81F9-2061B28FA609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19D66320-E9C8-4F21-91BD-0462B70F2F73}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8031204A-EDC0-4716-B806-54602A0267C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{AD0087DB-B3CF-424F-A3B1-CF03AF7D857B}"/>
+    <workbookView xWindow="76680" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{AD0087DB-B3CF-424F-A3B1-CF03AF7D857B}"/>
   </bookViews>
   <sheets>
     <sheet name="Import data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
   <si>
     <t>Basic parameters</t>
   </si>
@@ -316,13 +316,16 @@
   </si>
   <si>
     <t>Bidirectional</t>
+  </si>
+  <si>
+    <t>PLANPLC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,7 +458,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad 2" xfId="2" xr:uid="{6EBCB6DF-5D5B-44F9-B8EE-D92487182617}"/>
-    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{265E8CEA-DE9E-4F46-9615-8C18A90BAEDF}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -774,44 +777,44 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" style="9"/>
+    <col min="32" max="32" width="9.1796875" style="9"/>
     <col min="35" max="36" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -857,7 +860,7 @@
       </c>
       <c r="AJ1" s="3"/>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -983,25 +986,25 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" customHeight="1">
+    <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>40</v>
       </c>
@@ -1016,7 +1019,7 @@
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1041,11 +1044,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>41</v>
       </c>
@@ -1070,7 +1073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>47</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>53</v>
       </c>
@@ -1116,7 +1119,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>57</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>61</v>
       </c>
@@ -1152,9 +1155,11 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="K8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>63</v>
       </c>
@@ -1171,7 +1176,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>65</v>
       </c>
@@ -1188,132 +1193,132 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="E16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="5:5">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="5:5">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="5:5">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="5:5">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="5:5">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="5:5">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="5:5">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="5:5">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E24" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="5:5">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E25" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="5:5">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="5:5">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E27" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="5:5">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E28" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="5:5">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="5:5">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E30" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="5:5">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="5:5">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E32" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="5:5">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E33" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="5:5">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E34" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="5:5">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="5:5">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E36" t="s">
         <v>92</v>
       </c>

</xml_diff>